<commit_message>
Modificados documentos: Diagrama de Gantt y Presentación Proyecto.
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt - Juego.xlsx
+++ b/Diagrama de Gantt - Juego.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="107">
   <si>
     <t xml:space="preserve">DIAGRAMA DE GANTT previsión.</t>
   </si>
@@ -390,6 +390,9 @@
       </rPr>
       <t xml:space="preserve">Solo hemos adaptado ligeramente los iniciales</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Subir a GITHub los ejecutables junto con el código. Solo GNU/Linux.</t>
   </si>
   <si>
     <r>
@@ -1100,7 +1103,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1477,6 +1480,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="172" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1562,10 +1569,10 @@
   <dimension ref="A1:AMJ111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="C34:C35 G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.09"/>
@@ -6930,10 +6937,10 @@
   <dimension ref="A1:CO111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C34:C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.09"/>
@@ -10959,8 +10966,8 @@
       <c r="A35" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="45" t="s">
-        <v>83</v>
+      <c r="B35" s="94" t="s">
+        <v>103</v>
       </c>
       <c r="C35" s="45" t="s">
         <v>54</v>
@@ -10976,7 +10983,7 @@
         <v>5</v>
       </c>
       <c r="G35" s="93" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="H35" s="61"/>
       <c r="I35" s="65"/>
@@ -11279,7 +11286,7 @@
         <v>43135</v>
       </c>
       <c r="B38" s="45" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C38" s="45" t="s">
         <v>54</v>
@@ -11389,7 +11396,7 @@
         <v>43163</v>
       </c>
       <c r="B39" s="45" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C39" s="45" t="s">
         <v>54</v>
@@ -11598,7 +11605,7 @@
         <v>89</v>
       </c>
       <c r="B41" s="73" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C41" s="73" t="s">
         <v>54</v>
@@ -11613,7 +11620,7 @@
         <f aca="false">DAYS360(D41,E41)+1</f>
         <v>1</v>
       </c>
-      <c r="G41" s="94" t="n">
+      <c r="G41" s="95" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="66"/>
@@ -12055,7 +12062,7 @@
         <f aca="false">DAYS360(D45,E45)+1</f>
         <v>1</v>
       </c>
-      <c r="G45" s="94" t="n">
+      <c r="G45" s="95" t="n">
         <v>0</v>
       </c>
       <c r="H45" s="61"/>

</xml_diff>

<commit_message>
Modificado documento: Diagrama de Gantt.
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt - Juego.xlsx
+++ b/Diagrama de Gantt - Juego.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Previsión" sheetId="1" state="visible" r:id="rId2"/>
@@ -1605,11 +1605,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.09"/>
@@ -2907,10 +2907,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="46" t="n">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="E10" s="46" t="n">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="F10" s="47" t="n">
         <f aca="false">DAYS360(D10,E10)+1</f>
@@ -3014,10 +3014,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="46" t="n">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="E11" s="46" t="n">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F11" s="47" t="n">
         <f aca="false">DAYS360(D11,E11)+1</f>
@@ -3121,10 +3121,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="46" t="n">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="E12" s="46" t="n">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F12" s="47" t="n">
         <f aca="false">DAYS360(D12,E12)+1</f>
@@ -3228,10 +3228,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="46" t="n">
-        <v>43870</v>
+        <v>43899</v>
       </c>
       <c r="E13" s="46" t="n">
-        <v>43870</v>
+        <v>43899</v>
       </c>
       <c r="F13" s="47" t="n">
         <f aca="false">DAYS360(D13,E13)+1</f>
@@ -3335,10 +3335,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="46" t="n">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="E14" s="46" t="n">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="F14" s="47" t="n">
         <f aca="false">DAYS360(D14,E14)+1</f>
@@ -3540,10 +3540,10 @@
         <v>54</v>
       </c>
       <c r="D16" s="46" t="n">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="E16" s="46" t="n">
-        <v>43872</v>
+        <v>43901</v>
       </c>
       <c r="F16" s="47" t="n">
         <f aca="false">DAYS360(D16,E16)+1</f>
@@ -3647,10 +3647,10 @@
         <v>54</v>
       </c>
       <c r="D17" s="46" t="n">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="E17" s="46" t="n">
-        <v>43874</v>
+        <v>43903</v>
       </c>
       <c r="F17" s="47" t="n">
         <f aca="false">DAYS360(D17,E17)+1</f>
@@ -3754,10 +3754,10 @@
         <v>54</v>
       </c>
       <c r="D18" s="46" t="n">
-        <v>43877</v>
+        <v>43906</v>
       </c>
       <c r="E18" s="46" t="n">
-        <v>43881</v>
+        <v>43910</v>
       </c>
       <c r="F18" s="47" t="n">
         <f aca="false">DAYS360(D18,E18)+1</f>
@@ -3861,10 +3861,10 @@
         <v>54</v>
       </c>
       <c r="D19" s="46" t="n">
-        <v>43877</v>
+        <v>43906</v>
       </c>
       <c r="E19" s="46" t="n">
-        <v>43881</v>
+        <v>43910</v>
       </c>
       <c r="F19" s="47" t="n">
         <f aca="false">DAYS360(D19,E19)+1</f>
@@ -3968,14 +3968,14 @@
         <v>54</v>
       </c>
       <c r="D20" s="46" t="n">
-        <v>43877</v>
+        <v>43906</v>
       </c>
       <c r="E20" s="46" t="n">
-        <v>43907</v>
+        <v>43914</v>
       </c>
       <c r="F20" s="47" t="n">
         <f aca="false">DAYS360(D20,E20)+1</f>
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="G20" s="61"/>
       <c r="H20" s="65"/>
@@ -4075,14 +4075,14 @@
         <v>54</v>
       </c>
       <c r="D21" s="46" t="n">
-        <v>43877</v>
+        <v>43906</v>
       </c>
       <c r="E21" s="46" t="n">
         <v>43966</v>
       </c>
       <c r="F21" s="47" t="n">
         <f aca="false">DAYS360(D21,E21)+1</f>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G21" s="61"/>
       <c r="H21" s="65"/>
@@ -6973,11 +6973,11 @@
   </sheetPr>
   <dimension ref="A1:CO111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CH43" activeCellId="0" sqref="CH43"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.09"/>
@@ -8170,7 +8170,7 @@
       <c r="CN8" s="40"/>
       <c r="CO8" s="22"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="9" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A9" s="44" t="s">
         <v>40</v>
       </c>
@@ -8291,10 +8291,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="46" t="n">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="E10" s="46" t="n">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="F10" s="47" t="n">
         <f aca="false">DAYS360(D10,E10)+1</f>
@@ -8390,7 +8390,7 @@
       <c r="CN10" s="64"/>
       <c r="CO10" s="59"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="11" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A11" s="44" t="s">
         <v>44</v>
       </c>
@@ -8401,10 +8401,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="46" t="n">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="E11" s="46" t="n">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F11" s="47" t="n">
         <f aca="false">DAYS360(D11,E11)+1</f>
@@ -8500,7 +8500,7 @@
       <c r="CN11" s="64"/>
       <c r="CO11" s="59"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="12" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A12" s="44" t="s">
         <v>46</v>
       </c>
@@ -8511,10 +8511,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="46" t="n">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="E12" s="46" t="n">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F12" s="47" t="n">
         <f aca="false">DAYS360(D12,E12)+1</f>
@@ -8621,10 +8621,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="46" t="n">
-        <v>43870</v>
+        <v>43899</v>
       </c>
       <c r="E13" s="46" t="n">
-        <v>43870</v>
+        <v>43899</v>
       </c>
       <c r="F13" s="47" t="n">
         <f aca="false">DAYS360(D13,E13)+1</f>
@@ -8720,7 +8720,7 @@
       <c r="CN13" s="64"/>
       <c r="CO13" s="59"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="14" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A14" s="60" t="s">
         <v>50</v>
       </c>
@@ -8731,10 +8731,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="46" t="n">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="E14" s="46" t="n">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="F14" s="47" t="n">
         <f aca="false">DAYS360(D14,E14)+1</f>
@@ -8940,10 +8940,10 @@
         <v>54</v>
       </c>
       <c r="D16" s="46" t="n">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="E16" s="46" t="n">
-        <v>43872</v>
+        <v>43901</v>
       </c>
       <c r="F16" s="47" t="n">
         <f aca="false">DAYS360(D16,E16)+1</f>
@@ -9050,10 +9050,10 @@
         <v>54</v>
       </c>
       <c r="D17" s="46" t="n">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="E17" s="46" t="n">
-        <v>43874</v>
+        <v>43903</v>
       </c>
       <c r="F17" s="47" t="n">
         <f aca="false">DAYS360(D17,E17)+1</f>
@@ -9160,10 +9160,10 @@
         <v>54</v>
       </c>
       <c r="D18" s="46" t="n">
-        <v>43877</v>
+        <v>43906</v>
       </c>
       <c r="E18" s="46" t="n">
-        <v>43881</v>
+        <v>43910</v>
       </c>
       <c r="F18" s="47" t="n">
         <f aca="false">DAYS360(D18,E18)+1</f>
@@ -9270,10 +9270,10 @@
         <v>54</v>
       </c>
       <c r="D19" s="46" t="n">
-        <v>43877</v>
+        <v>43906</v>
       </c>
       <c r="E19" s="46" t="n">
-        <v>43881</v>
+        <v>43910</v>
       </c>
       <c r="F19" s="47" t="n">
         <f aca="false">DAYS360(D19,E19)+1</f>
@@ -9380,14 +9380,14 @@
         <v>54</v>
       </c>
       <c r="D20" s="46" t="n">
-        <v>43877</v>
+        <v>43906</v>
       </c>
       <c r="E20" s="46" t="n">
-        <v>43907</v>
+        <v>43914</v>
       </c>
       <c r="F20" s="47" t="n">
         <f aca="false">DAYS360(D20,E20)+1</f>
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="G20" s="86" t="n">
         <v>1</v>
@@ -9490,14 +9490,14 @@
         <v>54</v>
       </c>
       <c r="D21" s="46" t="n">
-        <v>43877</v>
+        <v>43906</v>
       </c>
       <c r="E21" s="46" t="n">
         <v>43966</v>
       </c>
       <c r="F21" s="47" t="n">
         <f aca="false">DAYS360(D21,E21)+1</f>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G21" s="86" t="n">
         <v>1</v>
@@ -9699,7 +9699,7 @@
       <c r="CN22" s="64"/>
       <c r="CO22" s="59"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="23" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A23" s="44" t="n">
         <v>44044</v>
       </c>

</xml_diff>